<commit_message>
Cambio lijero de tamaño en las columnas y filas
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de sprint aleph.xlsx
+++ b/Documentacion/Plan de sprint aleph.xlsx
@@ -380,17 +380,53 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF171717"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
@@ -424,6 +460,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -439,8 +482,23 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,29 +508,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -491,19 +526,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -522,10 +549,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -537,15 +572,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,14 +598,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,37 +660,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,6 +697,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,7 +726,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,7 +744,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +786,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,31 +810,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,43 +828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,21 +1060,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1059,6 +1080,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1089,6 +1125,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1097,105 +1157,81 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1204,74 +1240,74 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1425,10 +1461,145 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1764,1194 +1935,1194 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.74666666666667" customWidth="1"/>
+    <col min="1" max="1" width="6.75" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="7.4" customWidth="1"/>
-    <col min="4" max="4" width="9.10666666666667" customWidth="1"/>
-    <col min="5" max="5" width="8.74666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.10833333333333" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
     <col min="7" max="7" width="6.8" customWidth="1"/>
     <col min="8" max="8" width="12.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="7.4" customWidth="1"/>
-    <col min="10" max="10" width="8.88666666666667" customWidth="1"/>
-    <col min="11" max="11" width="8.62666666666667" customWidth="1"/>
-    <col min="12" max="12" width="8.62" customWidth="1"/>
+    <col min="10" max="10" width="8.88333333333333" customWidth="1"/>
+    <col min="11" max="11" width="8.625" customWidth="1"/>
+    <col min="12" max="12" width="8.61666666666667" customWidth="1"/>
     <col min="13" max="13" width="6.8" customWidth="1"/>
-    <col min="14" max="14" width="14.44" customWidth="1"/>
+    <col min="14" max="14" width="14.4416666666667" customWidth="1"/>
     <col min="15" max="15" width="7.4" customWidth="1"/>
-    <col min="16" max="16" width="8.54666666666667" customWidth="1"/>
+    <col min="16" max="16" width="8.55" customWidth="1"/>
     <col min="17" max="17" width="8.33333333333333" customWidth="1"/>
-    <col min="18" max="18" width="8.74666666666667" customWidth="1"/>
+    <col min="18" max="18" width="8.75" customWidth="1"/>
     <col min="19" max="19" width="6.8" customWidth="1"/>
-    <col min="20" max="20" width="13.5466666666667" customWidth="1"/>
+    <col min="20" max="20" width="13.55" customWidth="1"/>
     <col min="21" max="21" width="7.4" customWidth="1"/>
     <col min="22" max="22" width="9" customWidth="1"/>
-    <col min="23" max="23" width="8.87333333333333" customWidth="1"/>
-    <col min="24" max="24" width="8.74666666666667" customWidth="1"/>
-    <col min="26" max="26" width="41.8866666666667" customWidth="1"/>
+    <col min="23" max="23" width="8.875" customWidth="1"/>
+    <col min="24" max="24" width="8.75" customWidth="1"/>
+    <col min="26" max="26" width="41.8833333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:24">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="15.75" spans="1:24">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="24" t="s">
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="33" t="s">
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
     </row>
     <row r="2" ht="26.25" spans="1:24">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="S2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="34" t="s">
+      <c r="T2" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="34" t="s">
+      <c r="U2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="34" t="s">
+      <c r="V2" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="34" t="s">
+      <c r="W2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="34" t="s">
+      <c r="X2" s="88" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="35" customHeight="1" spans="1:24">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="57">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="68">
         <v>5</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="15" t="s">
+      <c r="L3" s="78"/>
+      <c r="M3" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="70">
         <v>2</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="36" t="s">
+      <c r="R3" s="89"/>
+      <c r="S3" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="15">
+      <c r="V3" s="70">
         <v>2</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="41"/>
+      <c r="X3" s="95"/>
     </row>
-    <row r="4" ht="31.5" spans="1:24">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="47.25" spans="1:24">
+      <c r="A4" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="57">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="70">
         <v>8</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="15" t="s">
+      <c r="L4" s="79"/>
+      <c r="M4" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="70">
         <v>5</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="36" t="s">
+      <c r="R4" s="89"/>
+      <c r="S4" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="15" t="s">
+      <c r="U4" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="70">
         <v>5</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="X4" s="41"/>
+      <c r="X4" s="95"/>
     </row>
-    <row r="5" ht="31.5" spans="1:24">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="47.25" spans="1:24">
+      <c r="A5" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="57">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="70">
         <v>5</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="15" t="s">
+      <c r="L5" s="79"/>
+      <c r="M5" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="70">
         <v>12</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36" t="s">
+      <c r="R5" s="89"/>
+      <c r="S5" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="T5" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="U5" s="15" t="s">
+      <c r="U5" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V5" s="15">
+      <c r="V5" s="70">
         <v>5</v>
       </c>
-      <c r="W5" s="15" t="s">
+      <c r="W5" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="41"/>
+      <c r="X5" s="95"/>
     </row>
     <row r="6" ht="34" customHeight="1" spans="1:24">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="57">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="67"/>
+      <c r="G6" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="70">
         <v>2</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="15" t="s">
+      <c r="L6" s="79"/>
+      <c r="M6" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="70">
         <v>2</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36" t="s">
+      <c r="R6" s="89"/>
+      <c r="S6" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="21" t="s">
+      <c r="T6" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="15" t="s">
+      <c r="U6" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="70">
         <v>2</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="41"/>
+      <c r="X6" s="95"/>
     </row>
     <row r="7" ht="35" customHeight="1" spans="1:24">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="57">
         <v>8</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="67"/>
+      <c r="G7" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="70">
         <v>5</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="15" t="s">
+      <c r="L7" s="79"/>
+      <c r="M7" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="70">
         <v>2</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36" t="s">
+      <c r="R7" s="89"/>
+      <c r="S7" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="U7" s="15" t="s">
+      <c r="U7" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="15">
+      <c r="V7" s="70">
         <v>2</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="41"/>
+      <c r="X7" s="95"/>
     </row>
     <row r="8" ht="35" customHeight="1" spans="1:24">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="57">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="70">
         <v>2</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="15" t="s">
+      <c r="L8" s="79"/>
+      <c r="M8" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="70">
         <v>5</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="Q8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36" t="s">
+      <c r="R8" s="89"/>
+      <c r="S8" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="15" t="s">
+      <c r="U8" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="70">
         <v>5</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="W8" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="41"/>
+      <c r="X8" s="95"/>
     </row>
     <row r="9" ht="35" customHeight="1" spans="1:24">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="15" t="s">
+      <c r="A9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="70">
         <v>12</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="15" t="s">
+      <c r="L9" s="79"/>
+      <c r="M9" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="70">
         <v>2</v>
       </c>
-      <c r="Q9" s="15" t="s">
+      <c r="Q9" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36" t="s">
+      <c r="R9" s="89"/>
+      <c r="S9" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="U9" s="15" t="s">
+      <c r="U9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V9" s="15">
+      <c r="V9" s="70">
         <v>5</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="X9" s="41"/>
+      <c r="X9" s="95"/>
     </row>
     <row r="10" ht="35" customHeight="1" spans="1:24">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="15" t="s">
+      <c r="A10" s="57"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="70">
         <v>2</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="R10" s="35"/>
-      <c r="S10" s="36" t="s">
+      <c r="R10" s="89"/>
+      <c r="S10" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="T10" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="U10" s="15" t="s">
+      <c r="U10" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V10" s="70">
         <v>8</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="X10" s="41"/>
+      <c r="X10" s="95"/>
     </row>
     <row r="11" ht="35" customHeight="1" spans="1:24">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="15" t="s">
+      <c r="A11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="70">
         <v>5</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="35"/>
-      <c r="S11" s="36" t="s">
+      <c r="R11" s="89"/>
+      <c r="S11" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="T11" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="15" t="s">
+      <c r="U11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="70">
         <v>2</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="W11" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="X11" s="41"/>
+      <c r="X11" s="95"/>
     </row>
     <row r="12" ht="35" customHeight="1" spans="1:24">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="15" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="70">
         <v>2</v>
       </c>
-      <c r="Q12" s="15" t="s">
+      <c r="Q12" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="R12" s="35"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="41"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="95"/>
     </row>
     <row r="13" ht="15.75" spans="1:24">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6">
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="60">
         <f>SUM(D3:D8)</f>
         <v>40</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7" t="s">
+      <c r="E13" s="60"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6">
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <f>SUM(J3:J9)</f>
         <v>39</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="7" t="s">
+      <c r="K13" s="60"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="6">
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <f>SUM(P3:P12)</f>
         <v>39</v>
       </c>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="7" t="s">
+      <c r="Q13" s="60"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="6">
+      <c r="T13" s="61"/>
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <f>SUM(V3:V11)</f>
         <v>36</v>
       </c>
-      <c r="W13" s="6"/>
-      <c r="X13" s="41"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="95"/>
     </row>
-    <row r="14" ht="17.25" spans="1:24">
-      <c r="A14" s="8" t="s">
+    <row r="14" ht="16.5" spans="1:24">
+      <c r="A14" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="24" t="s">
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="33" t="s">
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="33"/>
+      <c r="T14" s="87"/>
+      <c r="U14" s="87"/>
+      <c r="V14" s="87"/>
+      <c r="W14" s="87"/>
+      <c r="X14" s="87"/>
     </row>
     <row r="15" ht="39" customHeight="1" spans="1:24">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="17" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="15" t="s">
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="36" t="s">
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="3" t="s">
+      <c r="T15" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="42"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="96"/>
     </row>
     <row r="16" ht="39" customHeight="1" spans="1:24">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="15" t="s">
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="15" t="s">
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="36" t="s">
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="91"/>
+      <c r="S16" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="42"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60"/>
+      <c r="X16" s="96"/>
     </row>
     <row r="17" ht="31" customHeight="1" spans="1:24">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="15" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="15" t="s">
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="36" t="s">
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="91"/>
+      <c r="S17" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="42"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="60"/>
+      <c r="W17" s="60"/>
+      <c r="X17" s="96"/>
     </row>
     <row r="18" ht="41" customHeight="1" spans="1:24">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="15" t="s">
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="15" t="s">
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="36" t="s">
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="91"/>
+      <c r="S18" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="42"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="96"/>
     </row>
     <row r="19" ht="33" customHeight="1" spans="1:24">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="15" t="s">
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="15" t="s">
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="36" t="s">
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="91"/>
+      <c r="S19" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="42"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
+      <c r="X19" s="96"/>
     </row>
     <row r="20" ht="35" customHeight="1" spans="1:24">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="15" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="15" t="s">
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N20" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="36" t="s">
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="60"/>
+      <c r="R20" s="91"/>
+      <c r="S20" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="T20" s="6" t="s">
+      <c r="T20" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="42"/>
+      <c r="U20" s="60"/>
+      <c r="V20" s="60"/>
+      <c r="W20" s="60"/>
+      <c r="X20" s="96"/>
     </row>
     <row r="21" ht="41" customHeight="1" spans="1:24">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="15" t="s">
+      <c r="A21" s="57"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="15" t="s">
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="36" t="s">
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="91"/>
+      <c r="S21" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="T21" s="6" t="s">
+      <c r="T21" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="42"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="96"/>
     </row>
     <row r="22" ht="50" customHeight="1" spans="1:24">
-      <c r="A22" s="3"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="15" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="36" t="s">
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="91"/>
+      <c r="S22" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="T22" s="6" t="s">
+      <c r="T22" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="42"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="96"/>
     </row>
     <row r="23" ht="32" customHeight="1" spans="1:24">
-      <c r="A23" s="3"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="15" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="36" t="s">
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="91"/>
+      <c r="S23" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="T23" s="6" t="s">
+      <c r="T23" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="42"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="96"/>
     </row>
     <row r="24" ht="43" customHeight="1" spans="1:24">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="31" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="N24" s="32" t="s">
+      <c r="N24" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="40"/>
-      <c r="X24" s="43"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="86"/>
+      <c r="R24" s="92"/>
+      <c r="S24" s="93"/>
+      <c r="T24" s="94"/>
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="94"/>
+      <c r="X24" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -3013,44 +3184,46 @@
   <sheetPr/>
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.74666666666667" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="7.4" customWidth="1"/>
-    <col min="4" max="4" width="8.87333333333333" customWidth="1"/>
-    <col min="5" max="5" width="9.10666666666667" customWidth="1"/>
-    <col min="6" max="6" width="8.74666666666667" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="7.34166666666667" customWidth="1"/>
+    <col min="2" max="2" width="11.7166666666667" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="9.525" customWidth="1"/>
+    <col min="5" max="5" width="9.68333333333333" customWidth="1"/>
+    <col min="6" max="6" width="9.53333333333333" customWidth="1"/>
+    <col min="7" max="7" width="8.9" customWidth="1"/>
     <col min="8" max="8" width="6.8" customWidth="1"/>
     <col min="9" max="9" width="12.6666666666667" customWidth="1"/>
-    <col min="10" max="10" width="7.4" customWidth="1"/>
-    <col min="11" max="11" width="9.24666666666667" customWidth="1"/>
-    <col min="12" max="12" width="8.88666666666667" customWidth="1"/>
-    <col min="13" max="13" width="8.62666666666667" customWidth="1"/>
-    <col min="14" max="14" width="8.62" customWidth="1"/>
+    <col min="10" max="10" width="8.44166666666667" customWidth="1"/>
+    <col min="11" max="11" width="9.25" customWidth="1"/>
+    <col min="12" max="12" width="9.36666666666667" customWidth="1"/>
+    <col min="13" max="13" width="9.05833333333333" customWidth="1"/>
+    <col min="14" max="14" width="9.84166666666667" customWidth="1"/>
     <col min="15" max="15" width="6.8" customWidth="1"/>
-    <col min="16" max="16" width="14.44" customWidth="1"/>
-    <col min="17" max="17" width="7.4" customWidth="1"/>
-    <col min="18" max="18" width="8.87333333333333" customWidth="1"/>
-    <col min="19" max="19" width="8.54666666666667" customWidth="1"/>
-    <col min="20" max="20" width="8.33333333333333" customWidth="1"/>
-    <col min="21" max="21" width="8.74666666666667" customWidth="1"/>
+    <col min="16" max="16" width="14.4416666666667" customWidth="1"/>
+    <col min="17" max="17" width="7.80833333333333" customWidth="1"/>
+    <col min="18" max="18" width="9.21666666666667" customWidth="1"/>
+    <col min="19" max="19" width="9.375" customWidth="1"/>
+    <col min="20" max="21" width="9.21666666666667" customWidth="1"/>
     <col min="22" max="22" width="6.8" customWidth="1"/>
-    <col min="23" max="23" width="13.5466666666667" customWidth="1"/>
-    <col min="24" max="24" width="7.4" customWidth="1"/>
-    <col min="25" max="25" width="8.87333333333333" customWidth="1"/>
-    <col min="26" max="26" width="9" customWidth="1"/>
-    <col min="27" max="27" width="8.87333333333333" customWidth="1"/>
-    <col min="28" max="28" width="8.74666666666667" customWidth="1"/>
+    <col min="23" max="23" width="13.55" customWidth="1"/>
+    <col min="24" max="24" width="7.80833333333333" customWidth="1"/>
+    <col min="25" max="25" width="9.525" customWidth="1"/>
+    <col min="26" max="26" width="9.375" customWidth="1"/>
+    <col min="27" max="27" width="9.53333333333333" customWidth="1"/>
+    <col min="28" max="28" width="9.375" customWidth="1"/>
     <col min="29" max="29" width="6.8" customWidth="1"/>
     <col min="30" max="30" width="18.5" customWidth="1"/>
-    <col min="31" max="31" width="7.4" customWidth="1"/>
-    <col min="32" max="33" width="8.99333333333333" customWidth="1"/>
+    <col min="31" max="31" width="7.80833333333333" customWidth="1"/>
+    <col min="32" max="32" width="9.525" customWidth="1"/>
+    <col min="33" max="33" width="9.21666666666667" customWidth="1"/>
+    <col min="34" max="34" width="9.375" customWidth="1"/>
+    <col min="35" max="35" width="9.53333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:35">
@@ -3207,7 +3380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="35" customHeight="1" spans="1:35">
+    <row r="3" ht="55" customHeight="1" spans="1:35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -3296,9 +3469,9 @@
       <c r="AH3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="AI3" s="51"/>
+      <c r="AI3" s="52"/>
     </row>
-    <row r="4" ht="32.25" spans="1:35">
+    <row r="4" ht="27.75" spans="1:35">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -3387,9 +3560,9 @@
       <c r="AH4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AI4" s="51"/>
+      <c r="AI4" s="52"/>
     </row>
-    <row r="5" ht="31.5" spans="1:35">
+    <row r="5" ht="57" customHeight="1" spans="1:35">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -3478,9 +3651,9 @@
       <c r="AH5" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="AI5" s="51"/>
+      <c r="AI5" s="52"/>
     </row>
-    <row r="6" ht="34" customHeight="1" spans="1:35">
+    <row r="6" ht="41" customHeight="1" spans="1:35">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -3567,7 +3740,7 @@
       <c r="AH6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="AI6" s="51"/>
+      <c r="AI6" s="52"/>
     </row>
     <row r="7" ht="35" customHeight="1" spans="1:35">
       <c r="A7" s="3" t="s">
@@ -3646,9 +3819,9 @@
       <c r="AF7" s="48"/>
       <c r="AG7" s="48"/>
       <c r="AH7" s="48"/>
-      <c r="AI7" s="51"/>
+      <c r="AI7" s="52"/>
     </row>
-    <row r="8" ht="35" customHeight="1" spans="1:35">
+    <row r="8" ht="46" customHeight="1" spans="1:35">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -3727,9 +3900,9 @@
       <c r="AF8" s="48"/>
       <c r="AG8" s="48"/>
       <c r="AH8" s="48"/>
-      <c r="AI8" s="51"/>
+      <c r="AI8" s="52"/>
     </row>
-    <row r="9" ht="35" customHeight="1" spans="1:35">
+    <row r="9" ht="45" customHeight="1" spans="1:35">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -3784,9 +3957,9 @@
       <c r="AF9" s="48"/>
       <c r="AG9" s="48"/>
       <c r="AH9" s="48"/>
-      <c r="AI9" s="51"/>
+      <c r="AI9" s="52"/>
     </row>
-    <row r="10" ht="35" customHeight="1" spans="1:35">
+    <row r="10" ht="27" spans="1:35">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -3831,9 +4004,9 @@
       <c r="AF10" s="48"/>
       <c r="AG10" s="48"/>
       <c r="AH10" s="48"/>
-      <c r="AI10" s="51"/>
+      <c r="AI10" s="52"/>
     </row>
-    <row r="11" ht="35" customHeight="1" spans="1:35">
+    <row r="11" ht="27" spans="1:35">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -3878,9 +4051,9 @@
       <c r="AF11" s="48"/>
       <c r="AG11" s="48"/>
       <c r="AH11" s="48"/>
-      <c r="AI11" s="51"/>
+      <c r="AI11" s="52"/>
     </row>
-    <row r="12" ht="35" customHeight="1" spans="1:35">
+    <row r="12" ht="27" spans="1:35">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -3925,9 +4098,9 @@
       <c r="AF12" s="48"/>
       <c r="AG12" s="48"/>
       <c r="AH12" s="48"/>
-      <c r="AI12" s="51"/>
+      <c r="AI12" s="52"/>
     </row>
-    <row r="13" ht="35" customHeight="1" spans="1:35">
+    <row r="13" ht="40.5" spans="1:35">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -3972,9 +4145,9 @@
       <c r="AF13" s="48"/>
       <c r="AG13" s="48"/>
       <c r="AH13" s="48"/>
-      <c r="AI13" s="51"/>
+      <c r="AI13" s="52"/>
     </row>
-    <row r="14" ht="16.5" spans="1:35">
+    <row r="14" ht="14.25" spans="1:35">
       <c r="A14" s="7" t="s">
         <v>82</v>
       </c>
@@ -4049,9 +4222,9 @@
         <v>0</v>
       </c>
       <c r="AH14" s="50"/>
-      <c r="AI14" s="52"/>
+      <c r="AI14" s="53"/>
     </row>
-    <row r="15" ht="17.25" spans="1:33">
+    <row r="15" ht="17.25" spans="1:35">
       <c r="A15" s="8" t="s">
         <v>83</v>
       </c>
@@ -4088,11 +4261,17 @@
       <c r="Z15" s="33"/>
       <c r="AA15" s="33"/>
       <c r="AB15" s="33"/>
-      <c r="AG15" t="s">
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="51"/>
+      <c r="AE15" s="51"/>
+      <c r="AF15" s="51"/>
+      <c r="AG15" s="54" t="s">
         <v>118</v>
       </c>
+      <c r="AH15" s="51"/>
+      <c r="AI15" s="51"/>
     </row>
-    <row r="16" ht="39" customHeight="1" spans="1:28">
+    <row r="16" ht="39" customHeight="1" spans="1:35">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -4137,8 +4316,15 @@
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="42"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="51"/>
+      <c r="AE16" s="51"/>
+      <c r="AF16" s="51"/>
+      <c r="AG16" s="51"/>
+      <c r="AH16" s="51"/>
+      <c r="AI16" s="51"/>
     </row>
-    <row r="17" ht="39" customHeight="1" spans="1:28">
+    <row r="17" ht="39" customHeight="1" spans="1:35">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
@@ -4183,8 +4369,15 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="42"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51"/>
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
     </row>
-    <row r="18" ht="31" customHeight="1" spans="1:28">
+    <row r="18" ht="31" customHeight="1" spans="1:35">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -4229,8 +4422,15 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="42"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="51"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="51"/>
+      <c r="AI18" s="51"/>
     </row>
-    <row r="19" ht="41" customHeight="1" spans="1:28">
+    <row r="19" ht="41" customHeight="1" spans="1:35">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -4275,8 +4475,15 @@
       <c r="Z19" s="6"/>
       <c r="AA19" s="6"/>
       <c r="AB19" s="42"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="51"/>
+      <c r="AI19" s="51"/>
     </row>
-    <row r="20" ht="33" customHeight="1" spans="1:28">
+    <row r="20" ht="33" customHeight="1" spans="1:35">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -4321,8 +4528,15 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
       <c r="AB20" s="42"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
     </row>
-    <row r="21" ht="35" customHeight="1" spans="1:28">
+    <row r="21" ht="35" customHeight="1" spans="1:35">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -4367,8 +4581,15 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="42"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51"/>
+      <c r="AF21" s="51"/>
+      <c r="AG21" s="51"/>
+      <c r="AH21" s="51"/>
+      <c r="AI21" s="51"/>
     </row>
-    <row r="22" ht="41" customHeight="1" spans="1:28">
+    <row r="22" ht="41" customHeight="1" spans="1:35">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -4409,8 +4630,15 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="42"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="51"/>
+      <c r="AE22" s="51"/>
+      <c r="AF22" s="51"/>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="51"/>
+      <c r="AI22" s="51"/>
     </row>
-    <row r="23" ht="50" customHeight="1" spans="1:28">
+    <row r="23" ht="50" customHeight="1" spans="1:35">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -4445,8 +4673,15 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="42"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="51"/>
+      <c r="AI23" s="51"/>
     </row>
-    <row r="24" ht="32" customHeight="1" spans="1:28">
+    <row r="24" ht="32" customHeight="1" spans="1:35">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -4483,8 +4718,15 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="42"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="51"/>
+      <c r="AF24" s="51"/>
+      <c r="AG24" s="51"/>
+      <c r="AH24" s="51"/>
+      <c r="AI24" s="51"/>
     </row>
-    <row r="25" ht="43" customHeight="1" spans="1:28">
+    <row r="25" ht="43" customHeight="1" spans="1:35">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -4517,6 +4759,13 @@
       <c r="Z25" s="40"/>
       <c r="AA25" s="40"/>
       <c r="AB25" s="43"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="51"/>
+      <c r="AI25" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="49">

</xml_diff>

<commit_message>
Correccion de stories y se colocó tiempos reales de los stories terminados
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de sprint aleph.xlsx
+++ b/Documentacion/Plan de sprint aleph.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="123">
   <si>
     <t>SPRINT 1</t>
   </si>
@@ -392,10 +392,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -473,23 +473,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,8 +523,78 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -533,84 +608,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,13 +679,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,55 +739,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,19 +763,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,67 +841,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,21 +1144,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1185,15 +1170,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1207,6 +1183,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1225,153 +1216,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3307,7 +3307,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H3" sqref="H3:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -4969,8 +4969,8 @@
   <sheetPr/>
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -5220,11 +5220,15 @@
       <c r="R3" s="25">
         <v>5</v>
       </c>
-      <c r="S3" s="25"/>
+      <c r="S3" s="25">
+        <v>12</v>
+      </c>
       <c r="T3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="36"/>
+      <c r="U3" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="V3" s="15" t="s">
         <v>32</v>
       </c>
@@ -5260,7 +5264,7 @@
       </c>
       <c r="AI3" s="53"/>
     </row>
-    <row r="4" ht="53" customHeight="1" spans="1:35">
+    <row r="4" ht="46" customHeight="1" spans="1:35">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -5315,11 +5319,15 @@
       <c r="R4" s="25">
         <v>8</v>
       </c>
-      <c r="S4" s="25"/>
+      <c r="S4" s="25">
+        <v>8</v>
+      </c>
       <c r="T4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="36"/>
+      <c r="U4" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="V4" s="15" t="s">
         <v>66</v>
       </c>
@@ -5377,12 +5385,24 @@
       <c r="G5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="14">
+        <v>5</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="N5" s="27"/>
       <c r="O5" s="25" t="s">
         <v>44</v>
@@ -5456,12 +5476,24 @@
         <v>29</v>
       </c>
       <c r="G6" s="13"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="15">
+        <v>8</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="N6" s="24"/>
       <c r="O6" s="25" t="s">
         <v>51</v>
@@ -5630,12 +5662,24 @@
       <c r="G8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="15">
+        <v>2</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="N8" s="24"/>
       <c r="O8" s="25" t="s">
         <v>38</v>
@@ -5967,7 +6011,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="6">
         <f>SUM(K3:K13)</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L14" s="6">
         <f>SUM(L3:L13)</f>
@@ -5986,7 +6030,7 @@
       </c>
       <c r="S14" s="33">
         <f>SUM(S3:S13)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T14" s="33"/>
       <c r="U14" s="36"/>

</xml_diff>

<commit_message>
Se Incertaron los dato en la base de datos
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de sprint aleph.xlsx
+++ b/Documentacion/Plan de sprint aleph.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="123">
   <si>
     <t>SPRINT 1</t>
   </si>
@@ -392,9 +392,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
@@ -480,7 +480,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,15 +508,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -525,17 +533,32 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -554,8 +577,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,49 +608,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,7 +679,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,13 +739,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,13 +769,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,13 +805,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,7 +823,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,97 +853,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,21 +1129,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1163,6 +1148,45 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1201,174 +1225,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4970,7 +4970,7 @@
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="AI3" s="53"/>
     </row>
-    <row r="4" ht="46" customHeight="1" spans="1:35">
+    <row r="4" ht="61" customHeight="1" spans="1:35">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -5420,7 +5420,9 @@
       <c r="T5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="U5" s="36"/>
+      <c r="U5" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="V5" s="15" t="s">
         <v>45</v>
       </c>
@@ -5511,7 +5513,9 @@
       <c r="T6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="U6" s="36"/>
+      <c r="U6" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="V6" s="15" t="s">
         <v>54</v>
       </c>
@@ -5697,7 +5701,9 @@
       <c r="T8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="36"/>
+      <c r="U8" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="V8" s="15" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Se actualizo el plan para indicar que se termino el story Generar hoja de excel con datos
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de sprint aleph.xlsx
+++ b/Documentacion/Plan de sprint aleph.xlsx
@@ -392,10 +392,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -473,21 +473,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,16 +494,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -539,6 +533,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -547,29 +549,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -585,17 +564,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,9 +578,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -685,7 +685,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,19 +709,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,13 +721,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,19 +757,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,37 +793,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,37 +835,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,6 +1129,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1143,6 +1158,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1152,17 +1182,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1170,8 +1196,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1194,34 +1220,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1230,76 +1230,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1308,22 +1308,28 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1332,46 +1338,40 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4970,7 +4970,7 @@
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>

</xml_diff>